<commit_message>
Edit excel sheet, modified time off remove time function
</commit_message>
<xml_diff>
--- a/CTBTeam/CTBTeam/InternHours.xlsx
+++ b/CTBTeam/CTBTeam/InternHours.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alna172906\Documents\visual studio 2015\Projects\CTBTeam\CTBTeam\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alna172906\Source\Repos\Alps_Website\CTBTeam\CTBTeam\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
   <si>
     <t>Project B</t>
   </si>
@@ -813,43 +813,51 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac">
-  <dimension ref="A1:B3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" rightToLeft="false">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="6"/>
     <col min="2" max="2" width="22.85546875" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row spans="1:2" x14ac:dyDescent="0.25" outlineLevel="0" r="2">
+      <c r="C1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4">
         <v>42775</v>
       </c>
-    </row>
-    <row outlineLevel="0" r="3">
-      <c r="A3" s="6" t="inlineStr">
-        <is>
-          <t>Austin Danaj</t>
-        </is>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>6</v>
       </c>
       <c r="B3" s="4">
         <v>42776</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Converted from Microsoft Excel to Microsoft Access. Need to remove excel sheet, once confirmed conversion. Added Access Database.
</commit_message>
<xml_diff>
--- a/CTBTeam/CTBTeam/InternHours.xlsx
+++ b/CTBTeam/CTBTeam/InternHours.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -18,7 +18,7 @@
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
@@ -266,6 +266,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -301,6 +318,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -464,7 +498,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
-        <v>42772</v>
+        <v>42786</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -877,7 +911,7 @@
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <f>Sheet1!A1</f>
-        <v>42772</v>
+        <v>42786</v>
       </c>
       <c r="B1" t="s">
         <v>9</v>

</xml_diff>